<commit_message>
change in adding status
</commit_message>
<xml_diff>
--- a/input/ocha_pop.xlsx
+++ b/input/ocha_pop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{2967BCDC-435B-4136-8E53-2E23EF27DFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A250B1A0-85F9-44CA-B88B-997703C4828B}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{2967BCDC-435B-4136-8E53-2E23EF27DFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1046640A-1E74-4B33-855F-883B8195F47A}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,49 +116,49 @@
     <t>Admin Pcode</t>
   </si>
   <si>
-    <t>Children (6-17)</t>
-  </si>
-  <si>
-    <t>Girls  (6-17)</t>
-  </si>
-  <si>
-    <t>Boys  (6-17)</t>
-  </si>
-  <si>
-    <t>Host -- Children (6-17)</t>
-  </si>
-  <si>
-    <t>Host -- Girls  (6-17)</t>
-  </si>
-  <si>
-    <t>Host -- Boys  (6-17)</t>
-  </si>
-  <si>
-    <t>IDP -- Children (6-17)</t>
-  </si>
-  <si>
-    <t>IDP -- Girls  (6-17)</t>
-  </si>
-  <si>
-    <t>IDP -- Boys  (6-17)</t>
-  </si>
-  <si>
-    <t>Returnees -- Children (6-17)</t>
-  </si>
-  <si>
-    <t>Returnees -- Girls  (6-17)</t>
-  </si>
-  <si>
-    <t>Returnees -- Boys  (6-17)</t>
-  </si>
-  <si>
-    <t>Refugees -- Children (6-17)</t>
-  </si>
-  <si>
-    <t>Refugees -- Girls  (6-17)</t>
-  </si>
-  <si>
-    <t>Refugees -- Boys  (6-17)</t>
+    <t>Children (5-17)</t>
+  </si>
+  <si>
+    <t>Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>Host -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Host -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Host -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>IDP -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>IDP -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>IDP -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>Returnees -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Returnees -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Returnees -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees -- Boys  (5-17)</t>
   </si>
 </sst>
 </file>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -579,6 +579,14 @@
         <f>C2*0.6</f>
         <v>60</v>
       </c>
+      <c r="F2">
+        <f>C2*0.7</f>
+        <v>70</v>
+      </c>
+      <c r="J2">
+        <f>C2*0.3</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
@@ -598,6 +606,14 @@
         <f t="shared" ref="E3:E12" si="1">C3*0.6</f>
         <v>90</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F25" si="2">C3*0.7</f>
+        <v>105</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J25" si="3">C3*0.3</f>
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
@@ -617,6 +633,14 @@
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
@@ -636,6 +660,14 @@
         <f t="shared" si="1"/>
         <v>78.599999999999994</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>91.699999999999989</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>39.299999999999997</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
@@ -655,6 +687,14 @@
         <f t="shared" si="1"/>
         <v>79.2</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>92.399999999999991</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>39.6</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
@@ -674,6 +714,14 @@
         <f t="shared" si="1"/>
         <v>79.8</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>93.1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>39.9</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
@@ -693,6 +741,14 @@
         <f t="shared" si="1"/>
         <v>80.399999999999991</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>93.8</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>40.199999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
@@ -712,6 +768,14 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>94.5</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>40.5</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
@@ -731,6 +795,14 @@
         <f t="shared" si="1"/>
         <v>81.599999999999994</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>95.199999999999989</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>40.799999999999997</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
@@ -750,6 +822,14 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
@@ -769,6 +849,14 @@
         <f t="shared" si="1"/>
         <v>82.8</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>96.6</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>41.4</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
@@ -788,6 +876,14 @@
         <f>C13*0.47</f>
         <v>65.33</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>97.3</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>41.699999999999996</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
@@ -800,12 +896,20 @@
         <v>140</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D25" si="2">C14*0.53</f>
+        <f t="shared" ref="D14:D25" si="4">C14*0.53</f>
         <v>74.2</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:E25" si="3">C14*0.47</f>
+        <f t="shared" ref="E14:E25" si="5">C14*0.47</f>
         <v>65.8</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.75">
@@ -819,12 +923,20 @@
         <v>141</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>74.73</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>66.27</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>98.699999999999989</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>42.3</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.75">
@@ -838,15 +950,23 @@
         <v>142</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>75.260000000000005</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>66.739999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>99.399999999999991</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -857,15 +977,23 @@
         <v>143</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>75.790000000000006</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.209999999999994</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>100.1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>42.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -876,15 +1004,23 @@
         <v>250</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>132.5</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>117.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -895,15 +1031,23 @@
         <v>145</v>
       </c>
       <c r="D19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>76.850000000000009</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>68.149999999999991</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>101.5</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -914,15 +1058,23 @@
         <v>146</v>
       </c>
       <c r="D20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>77.38000000000001</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>68.61999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>102.19999999999999</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -933,15 +1085,23 @@
         <v>147</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>77.910000000000011</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>69.089999999999989</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>102.89999999999999</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>44.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -952,15 +1112,23 @@
         <v>148</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78.44</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>69.56</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>103.6</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -971,15 +1139,23 @@
         <v>500</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>265</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>235</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>350</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -990,15 +1166,23 @@
         <v>150</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>79.5</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>70.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1009,12 +1193,20 @@
         <v>151</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>80.03</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>70.97</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>105.69999999999999</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>45.3</v>
       </c>
     </row>
   </sheetData>
@@ -1023,6 +1215,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100873D3DDBB405ED4AA6367858D626971E" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="480f6128cb4bbd073f6326125a41424c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6" xmlns:ns3="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="379a74a9217f9861f5630dd08d9dc250" ns2:_="" ns3:_="">
     <xsd:import namespace="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
@@ -1251,15 +1452,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1272,6 +1464,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9ABE00-1A66-40F4-8530-1F10CCD931C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1290,14 +1490,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACDE1998-78A0-4AB1-AFCD-9276514F0C55}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
change ocha pop figures. Adding 5YO!!!!!
</commit_message>
<xml_diff>
--- a/input/ocha_pop.xlsx
+++ b/input/ocha_pop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{59E61301-DE0E-4AD8-9E51-0BB6543F4157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B8DCE4C-0703-47A7-8354-99C2A55D7E17}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{59E61301-DE0E-4AD8-9E51-0BB6543F4157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C38C1C0E-C8F6-4EBB-92EA-DB26ABA8FC92}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>martina.vit</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{FCD418C9-AAAD-4616-95A6-D01897719AFB}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{56324F5C-D1A9-4D0C-8823-3368F6C4E332}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EEAD403E-24FC-4CB9-ACFE-7DE1EEFC0B71}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{7D552B87-B493-4001-B304-1964DC070B87}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>diinsoor</t>
   </si>
@@ -198,18 +198,6 @@
     <t>Returnees/Retournés -- Boys/Garcons (5-17)</t>
   </si>
   <si>
-    <t>Refugees/Refugiee -- Children/Enfants (5-17)</t>
-  </si>
-  <si>
-    <t>Refugees/Refugiee -- Girls/Filles (5-17)</t>
-  </si>
-  <si>
-    <t>Refugees/Refugiee -- Boys/Garcons (5-17)</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>ToT -- Children/Enfants (5-17)</t>
   </si>
   <si>
@@ -220,13 +208,34 @@
   </si>
   <si>
     <t>Host/Hôte -- Children/Enfants (5-17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5yo -- Children/Enfants  </t>
+  </si>
+  <si>
+    <t>5yo -- Girls/Filles</t>
+  </si>
+  <si>
+    <t>5yo -- Boys/Garcons</t>
+  </si>
+  <si>
+    <t>Refugees/Refugiees -- Children/Enfants (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees/Refugiees -- Girls/Filles (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees/Refugiees -- Boys/Garcons (5-17)</t>
+  </si>
+  <si>
+    <t>Other -- Children/Enfants (5-17)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,34 +244,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -280,8 +261,43 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,19 +306,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,8 +346,26 @@
         <bgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -370,76 +392,57 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -746,718 +749,823 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" s="14" customFormat="1" ht="39.35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="S1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>100000</v>
+      <c r="C2" s="1">
+        <v>295338.66666666669</v>
       </c>
       <c r="D2">
         <f>C2*0.4</f>
-        <v>40000</v>
+        <v>118135.46666666667</v>
       </c>
       <c r="E2">
         <f>C2*0.6</f>
-        <v>60000</v>
+        <v>177203.20000000001</v>
       </c>
       <c r="F2">
+        <f>C2*0.1</f>
+        <v>29533.866666666669</v>
+      </c>
+      <c r="I2">
         <f>C2*0.7</f>
-        <v>70000</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I25" si="0">C2*0.3</f>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
+        <v>206737.06666666668</v>
+      </c>
+      <c r="L2">
+        <f>C2*0.3</f>
+        <v>88601.600000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>150000</v>
+      <c r="C3" s="2">
+        <v>134467.33333333334</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D12" si="1">C3*0.4</f>
-        <v>60000</v>
+        <f t="shared" ref="D3:D12" si="0">C3*0.4</f>
+        <v>53786.933333333342</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E12" si="2">C3*0.6</f>
-        <v>90000</v>
+        <f t="shared" ref="E3:E12" si="1">C3*0.6</f>
+        <v>80680.400000000009</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F25" si="3">C3*0.7</f>
-        <v>105000</v>
+        <f>C3*0.11</f>
+        <v>14791.406666666668</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" ref="I3:I25" si="2">C3*0.7</f>
+        <v>94127.133333333331</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L25" si="3">C3*0.3</f>
+        <v>40340.200000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>130000</v>
+      <c r="C4" s="1">
+        <v>121822.66666666667</v>
       </c>
       <c r="D4">
+        <f t="shared" si="0"/>
+        <v>48729.066666666673</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="1"/>
-        <v>52000</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
-        <v>78000</v>
+        <v>73093.600000000006</v>
       </c>
       <c r="F4">
-        <f t="shared" si="3"/>
-        <v>91000</v>
+        <f t="shared" ref="F3:F25" si="4">C4*0.1</f>
+        <v>12182.266666666668</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>39000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>85275.866666666669</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>36546.800000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>131000</v>
+      <c r="C5" s="2">
+        <v>113367.33333333333</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>45346.933333333334</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="1"/>
-        <v>52400</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>78600</v>
+        <v>68020.399999999994</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
-        <v>91700</v>
+        <f>C5*0.12</f>
+        <v>13604.079999999998</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
-        <v>39300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>79357.133333333331</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>34010.199999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>132000</v>
+      <c r="C6" s="1">
+        <v>247962</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>99184.8</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="1"/>
-        <v>52800</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>79200</v>
+        <v>148777.19999999998</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
-        <v>92400</v>
+        <f t="shared" si="4"/>
+        <v>24796.2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
-        <v>39600</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>173573.4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>74388.599999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>133000</v>
+      <c r="C7" s="2">
+        <v>101572</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>40628.800000000003</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="1"/>
-        <v>53200</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>79800</v>
+        <v>60943.199999999997</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
-        <v>93100</v>
+        <f>C7*0.08</f>
+        <v>8125.76</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
-        <v>39900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>71100.399999999994</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>30471.599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>134000</v>
+      <c r="C8" s="1">
+        <v>147696</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>59078.400000000001</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="1"/>
-        <v>53600</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>80400</v>
+        <v>88617.599999999991</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
-        <v>93800</v>
+        <f t="shared" si="4"/>
+        <v>14769.6</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
-        <v>40200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>103387.2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>44308.799999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>135000</v>
+      <c r="C9" s="2">
+        <v>133947.33333333334</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>53578.933333333342</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="1"/>
-        <v>54000</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>81000</v>
+        <v>80368.400000000009</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
-        <v>94500</v>
+        <f t="shared" si="4"/>
+        <v>13394.733333333335</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
-        <v>40500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>93763.133333333331</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>40184.200000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>136000</v>
+      <c r="C10" s="1">
+        <v>342878.66666666669</v>
       </c>
       <c r="D10">
+        <f t="shared" si="0"/>
+        <v>137151.46666666667</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="1"/>
-        <v>54400</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>81600</v>
+        <v>205727.2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
-        <v>95200</v>
+        <f>C10*0.07</f>
+        <v>24001.506666666672</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
-        <v>40800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>240015.06666666665</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>102863.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>200000</v>
+      <c r="C11" s="2">
+        <v>70406.666666666672</v>
       </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>28162.666666666672</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="1"/>
-        <v>80000</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="2"/>
-        <v>120000</v>
+        <v>42244</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
-        <v>140000</v>
+        <f t="shared" si="4"/>
+        <v>7040.6666666666679</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>49284.666666666664</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>21122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>138000</v>
+      <c r="C12" s="1">
+        <v>670875.33333333337</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>268350.13333333336</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="1"/>
-        <v>55200</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="2"/>
-        <v>82800</v>
+        <v>402525.2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
-        <v>96600</v>
+        <f t="shared" si="4"/>
+        <v>67087.53333333334</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
-        <v>41400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>469612.73333333334</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>201262.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>139000</v>
+      <c r="C13" s="2">
+        <v>163046.66666666666</v>
       </c>
       <c r="D13">
         <f>C13*0.53</f>
-        <v>73670</v>
+        <v>86414.733333333337</v>
       </c>
       <c r="E13">
         <f>C13*0.47</f>
-        <v>65329.999999999993</v>
+        <v>76631.93333333332</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
-        <v>97300</v>
+        <f t="shared" si="4"/>
+        <v>16304.666666666666</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
-        <v>41700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>114132.66666666666</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>48913.999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>140000</v>
+      <c r="C14" s="1">
+        <v>134357.33333333334</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D25" si="4">C14*0.53</f>
-        <v>74200</v>
+        <f t="shared" ref="D14:D25" si="5">C14*0.53</f>
+        <v>71209.386666666673</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:E25" si="5">C14*0.47</f>
-        <v>65800</v>
+        <f t="shared" ref="E14:E25" si="6">C14*0.47</f>
+        <v>63147.94666666667</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
-        <v>98000</v>
+        <f>C14*0.11</f>
+        <v>14779.306666666667</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>94050.133333333331</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>40307.200000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>141000</v>
+      <c r="C15" s="2">
+        <v>116915.33333333333</v>
       </c>
       <c r="D15">
-        <f t="shared" si="4"/>
-        <v>74730</v>
+        <f t="shared" si="5"/>
+        <v>61965.126666666671</v>
       </c>
       <c r="E15">
-        <f t="shared" si="5"/>
-        <v>66270</v>
+        <f t="shared" si="6"/>
+        <v>54950.206666666658</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
-        <v>98700</v>
+        <f>C15*0.11</f>
+        <v>12860.686666666666</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
-        <v>42300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>81840.733333333323</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>35074.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>142000</v>
+      <c r="C16" s="1">
+        <v>111385.33333333333</v>
       </c>
       <c r="D16">
+        <f t="shared" si="5"/>
+        <v>59034.226666666669</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="6"/>
+        <v>52351.106666666659</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="4"/>
-        <v>75260</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="5"/>
-        <v>66740</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>99400</v>
+        <v>11138.533333333333</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
-        <v>42600</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>77969.733333333323</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>33415.599999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>143000</v>
+      <c r="C17" s="2">
+        <v>117686.66666666667</v>
       </c>
       <c r="D17">
-        <f t="shared" si="4"/>
-        <v>75790</v>
+        <f t="shared" si="5"/>
+        <v>62373.933333333342</v>
       </c>
       <c r="E17">
-        <f t="shared" si="5"/>
-        <v>67210</v>
+        <f t="shared" si="6"/>
+        <v>55312.73333333333</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
-        <v>100100</v>
+        <f>C17*0.1</f>
+        <v>11768.666666666668</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
-        <v>42900</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>82380.666666666672</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>35306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>250000</v>
+      <c r="C18" s="1">
+        <v>406036.66666666669</v>
       </c>
       <c r="D18">
-        <f t="shared" si="4"/>
-        <v>132500</v>
+        <f t="shared" si="5"/>
+        <v>215199.43333333335</v>
       </c>
       <c r="E18">
-        <f t="shared" si="5"/>
-        <v>117500</v>
+        <f t="shared" si="6"/>
+        <v>190837.23333333334</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
-        <v>175000</v>
+        <f>C18*0.13</f>
+        <v>52784.76666666667</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>284225.66666666669</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>121811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>145000</v>
+      <c r="C19" s="2">
+        <v>101086.66666666667</v>
       </c>
       <c r="D19">
-        <f t="shared" si="4"/>
-        <v>76850</v>
+        <f t="shared" si="5"/>
+        <v>53575.933333333342</v>
       </c>
       <c r="E19">
-        <f t="shared" si="5"/>
-        <v>68150</v>
+        <f t="shared" si="6"/>
+        <v>47510.73333333333</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
-        <v>101500</v>
+        <f t="shared" ref="F19:F21" si="7">C19*0.13</f>
+        <v>13141.266666666668</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
-        <v>43500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>70760.666666666672</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>30326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>146000</v>
+      <c r="C20" s="1">
+        <v>347286.66666666669</v>
       </c>
       <c r="D20">
-        <f t="shared" si="4"/>
-        <v>77380</v>
+        <f t="shared" si="5"/>
+        <v>184061.93333333335</v>
       </c>
       <c r="E20">
-        <f t="shared" si="5"/>
-        <v>68620</v>
+        <f t="shared" si="6"/>
+        <v>163224.73333333334</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
-        <v>102200</v>
+        <f t="shared" si="7"/>
+        <v>45147.26666666667</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>243100.66666666666</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>104186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>147000</v>
+      <c r="C21" s="2">
+        <v>141172</v>
       </c>
       <c r="D21">
-        <f t="shared" si="4"/>
-        <v>77910</v>
+        <f t="shared" si="5"/>
+        <v>74821.16</v>
       </c>
       <c r="E21">
-        <f t="shared" si="5"/>
-        <v>69090</v>
+        <f t="shared" si="6"/>
+        <v>66350.84</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
-        <v>102900</v>
+        <f t="shared" si="7"/>
+        <v>18352.36</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
-        <v>44100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>98820.4</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>42351.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>148000</v>
+      <c r="C22" s="1">
+        <v>166585.33333333334</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
-        <v>78440</v>
+        <f t="shared" si="5"/>
+        <v>88290.226666666669</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
-        <v>69560</v>
+        <f t="shared" si="6"/>
+        <v>78295.106666666674</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
-        <v>103600</v>
+        <f>C22*0.85</f>
+        <v>141597.53333333333</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
-        <v>44400</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>116609.73333333334</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>49975.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23">
-        <v>500000</v>
+      <c r="C23" s="2">
+        <v>165322.66666666666</v>
       </c>
       <c r="D23">
-        <f t="shared" si="4"/>
-        <v>265000</v>
+        <f t="shared" si="5"/>
+        <v>87621.013333333336</v>
       </c>
       <c r="E23">
-        <f t="shared" si="5"/>
-        <v>235000</v>
+        <f t="shared" si="6"/>
+        <v>77701.653333333321</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
-        <v>350000</v>
+        <f t="shared" ref="F23:F25" si="8">C23*0.85</f>
+        <v>140524.26666666666</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>115725.86666666665</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>49596.799999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>150000</v>
+      <c r="C24" s="1">
+        <v>107594.66666666667</v>
       </c>
       <c r="D24">
-        <f t="shared" si="4"/>
-        <v>79500</v>
+        <f t="shared" si="5"/>
+        <v>57025.17333333334</v>
       </c>
       <c r="E24">
-        <f t="shared" si="5"/>
-        <v>70500</v>
+        <f t="shared" si="6"/>
+        <v>50569.493333333332</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
-        <v>105000</v>
+        <f t="shared" si="8"/>
+        <v>91455.466666666674</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+        <f t="shared" si="2"/>
+        <v>75316.266666666663</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>32278.400000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>151000</v>
+      <c r="C25" s="3">
+        <v>116932</v>
       </c>
       <c r="D25">
-        <f t="shared" si="4"/>
-        <v>80030</v>
+        <f t="shared" si="5"/>
+        <v>61973.960000000006</v>
       </c>
       <c r="E25">
-        <f t="shared" si="5"/>
-        <v>70970</v>
+        <f t="shared" si="6"/>
+        <v>54958.039999999994</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
-        <v>105700</v>
+        <f t="shared" si="8"/>
+        <v>99392.2</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
-        <v>45300</v>
+        <f t="shared" si="2"/>
+        <v>81852.399999999994</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>35079.599999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1696,15 +1804,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" xsi:nil="true"/>
@@ -1713,6 +1812,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1735,14 +1843,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACDE1998-78A0-4AB1-AFCD-9276514F0C55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1757,4 +1857,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>